<commit_message>
feat: Add admin dashboard, forgot password, and updated sample DB
- Refactor index.html to dynamic rendering.
- Add admin.html with Login, Dashboard, and Forgot Password features.
- Implement 'Forgot Password' flow: resets password and emails it via GAS.
- Update GAS code (deployment/code.gs) to handle forgotPassword and token auth.
- Update Mock Data and Schema to include Email field for Users.
- Regenerate Excel sample database (deployment/isparmo_database_sample.xlsx) with correct columns.
- Provide detailed deployment guide (GUIDE_DEPLOYMENT.md).
</commit_message>
<xml_diff>
--- a/deployment/isparmo_database_sample.xlsx
+++ b/deployment/isparmo_database_sample.xlsx
@@ -511,7 +511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,11 @@
           <t>Password</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -540,6 +545,11 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>123456</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>admin@example.com</t>
         </is>
       </c>
     </row>

</xml_diff>